<commit_message>
Fixed db instance issue.
</commit_message>
<xml_diff>
--- a/test_files/synonyms_import_test_file.xlsx
+++ b/test_files/synonyms_import_test_file.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scratch\METRO MASTER\_ICS325_2017_Spring\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Name-in-Synonym_dolphins\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Synonyms" sheetId="1" r:id="rId1"/>
@@ -834,9 +834,6 @@
     <t>విశ్వం, జగత్తు, లోకం, ప్రపంచం, సర్వం</t>
   </si>
   <si>
-    <t>చిన్నపిల్ల –బాలిక</t>
-  </si>
-  <si>
     <t>దుంప, వేరు</t>
   </si>
   <si>
@@ -1267,13 +1264,16 @@
   </si>
   <si>
     <t>ఎగతాళి, వెక్కరింత</t>
+  </si>
+  <si>
+    <t>చిన్నపిల్ల, బాలిక</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1416,8 +1416,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1505,6 +1533,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1540,6 +1585,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1694,20 +1756,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B412"/>
   <sheetViews>
-    <sheetView topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="G417" sqref="G417"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.46484375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.53125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="7"/>
+    <col min="5" max="16384" width="8.86328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>94</v>
       </c>
@@ -1715,15 +1777,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1731,7 +1793,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1739,7 +1801,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1747,15 +1809,15 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.7">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1763,7 +1825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1771,7 +1833,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1779,7 +1841,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1787,15 +1849,15 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.7">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1803,15 +1865,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.7">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1819,7 +1881,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1827,7 +1889,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1835,7 +1897,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1843,15 +1905,15 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.7">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1859,15 +1921,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.7">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1875,7 +1937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1883,7 +1945,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1891,95 +1953,95 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="24" spans="1:2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.7">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.7">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.7">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.7">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.7">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.7">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.7">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.7">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.7">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.7">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.7">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -1987,23 +2049,23 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="36" spans="1:2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.7">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.7">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2011,7 +2073,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="39" spans="1:2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2019,7 +2081,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="40" spans="1:2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2027,7 +2089,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="41" spans="1:2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2035,7 +2097,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="42" spans="1:2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2043,23 +2105,23 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="43" spans="1:2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.7">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.7">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -2067,7 +2129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="46" spans="1:2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -2075,7 +2137,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="47" spans="1:2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -2083,7 +2145,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="48" spans="1:2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -2091,7 +2153,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="49" spans="1:2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -2099,7 +2161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="50" spans="1:2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2107,7 +2169,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="51" spans="1:2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -2115,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="52" spans="1:2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2123,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="53" spans="1:2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -2131,7 +2193,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="54" spans="1:2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -2139,7 +2201,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="55" spans="1:2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -2147,7 +2209,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="56" spans="1:2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -2155,7 +2217,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="57" spans="1:2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -2163,7 +2225,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="58" spans="1:2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -2171,7 +2233,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="59" spans="1:2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -2179,7 +2241,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="60" spans="1:2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -2187,7 +2249,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="61" spans="1:2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -2195,15 +2257,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="62" spans="1:2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.7">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -2211,7 +2273,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="64" spans="1:2">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -2219,7 +2281,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="65" spans="1:2">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -2227,7 +2289,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="66" spans="1:2">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -2235,7 +2297,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="67" spans="1:2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -2243,7 +2305,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="68" spans="1:2">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -2251,7 +2313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="69" spans="1:2">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -2259,7 +2321,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="70" spans="1:2">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -2267,7 +2329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="71" spans="1:2">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -2275,7 +2337,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="72" spans="1:2">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -2283,15 +2345,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="73" spans="1:2">
       <c r="A73" s="7">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.7">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -2299,15 +2361,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="75" spans="1:2">
       <c r="A75" s="7">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -2315,15 +2377,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="77" spans="1:2">
       <c r="A77" s="7">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.7">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -2331,7 +2393,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="79" spans="1:2">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -2339,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="80" spans="1:2">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -2347,7 +2409,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="81" spans="1:2">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -2355,7 +2417,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="82" spans="1:2">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -2363,7 +2425,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="83" spans="1:2">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -2371,7 +2433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="84" spans="1:2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -2379,7 +2441,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="85" spans="1:2">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -2387,7 +2449,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="86" spans="1:2">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -2395,7 +2457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="87" spans="1:2">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -2403,7 +2465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="88" spans="1:2">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -2411,71 +2473,71 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="89" spans="1:2">
       <c r="A89" s="7">
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" s="7">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.7">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" s="7">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.7">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" s="7">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.7">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.7">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" s="7">
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.7">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" s="7">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.7">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" s="7">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.7">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -2483,39 +2545,39 @@
         <v>86</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="98" spans="1:2">
       <c r="A98" s="7">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.7">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" s="7">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.7">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" s="7">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.7">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" s="7">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.7">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" s="7">
         <v>101</v>
       </c>
@@ -2523,15 +2585,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="103" spans="1:2">
       <c r="A103" s="7">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.7">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104" s="7">
         <v>103</v>
       </c>
@@ -2539,7 +2601,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="105" spans="1:2">
       <c r="A105" s="7">
         <v>104</v>
       </c>
@@ -2547,7 +2609,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="106" spans="1:2">
       <c r="A106" s="7">
         <v>105</v>
       </c>
@@ -2555,15 +2617,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="107" spans="1:2">
       <c r="A107" s="7">
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.7">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108" s="7">
         <v>107</v>
       </c>
@@ -2571,7 +2633,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="109" spans="1:2">
       <c r="A109" s="7">
         <v>108</v>
       </c>
@@ -2579,15 +2641,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="110" spans="1:2">
       <c r="A110" s="7">
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.7">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111" s="7">
         <v>110</v>
       </c>
@@ -2595,15 +2657,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="112" spans="1:2">
       <c r="A112" s="7">
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.7">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" s="7">
         <v>112</v>
       </c>
@@ -2611,15 +2673,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="114" spans="1:2">
       <c r="A114" s="7">
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.7">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" s="7">
         <v>114</v>
       </c>
@@ -2627,15 +2689,15 @@
         <v>204</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="116" spans="1:2">
       <c r="A116" s="7">
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" s="7">
         <v>116</v>
       </c>
@@ -2643,7 +2705,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="118" spans="1:2">
       <c r="A118" s="7">
         <v>117</v>
       </c>
@@ -2651,15 +2713,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="119" spans="1:2">
       <c r="A119" s="7">
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.7">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -2667,7 +2729,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="121" spans="1:2">
       <c r="A121" s="7">
         <v>120</v>
       </c>
@@ -2675,7 +2737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="122" spans="1:2">
       <c r="A122" s="7">
         <v>121</v>
       </c>
@@ -2683,15 +2745,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="123" spans="1:2">
       <c r="A123" s="7">
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.7">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124" s="7">
         <v>123</v>
       </c>
@@ -2699,7 +2761,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="125" spans="1:2">
       <c r="A125" s="7">
         <v>124</v>
       </c>
@@ -2707,7 +2769,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="126" spans="1:2">
       <c r="A126" s="7">
         <v>125</v>
       </c>
@@ -2715,7 +2777,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="127" spans="1:2">
       <c r="A127" s="7">
         <v>126</v>
       </c>
@@ -2723,7 +2785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="128" spans="1:2">
       <c r="A128" s="7">
         <v>127</v>
       </c>
@@ -2731,7 +2793,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="129" spans="1:2">
       <c r="A129" s="7">
         <v>128</v>
       </c>
@@ -2739,15 +2801,15 @@
         <v>201</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="130" spans="1:2">
       <c r="A130" s="7">
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.7">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131" s="7">
         <v>130</v>
       </c>
@@ -2755,7 +2817,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="132" spans="1:2">
       <c r="A132" s="7">
         <v>131</v>
       </c>
@@ -2763,7 +2825,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="133" spans="1:2">
       <c r="A133" s="7">
         <v>132</v>
       </c>
@@ -2771,7 +2833,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="134" spans="1:2">
       <c r="A134" s="7">
         <v>133</v>
       </c>
@@ -2779,7 +2841,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="135" spans="1:2">
       <c r="A135" s="7">
         <v>134</v>
       </c>
@@ -2787,7 +2849,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="136" spans="1:2">
       <c r="A136" s="7">
         <v>135</v>
       </c>
@@ -2795,7 +2857,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="137" spans="1:2">
       <c r="A137" s="7">
         <v>136</v>
       </c>
@@ -2803,7 +2865,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="138" spans="1:2">
       <c r="A138" s="7">
         <v>137</v>
       </c>
@@ -2811,7 +2873,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="139" spans="1:2">
       <c r="A139" s="7">
         <v>138</v>
       </c>
@@ -2819,7 +2881,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="140" spans="1:2">
       <c r="A140" s="7">
         <v>139</v>
       </c>
@@ -2827,7 +2889,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="141" spans="1:2">
       <c r="A141" s="7">
         <v>140</v>
       </c>
@@ -2835,7 +2897,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="142" spans="1:2">
       <c r="A142" s="7">
         <v>141</v>
       </c>
@@ -2843,23 +2905,23 @@
         <v>197</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="143" spans="1:2">
       <c r="A143" s="7">
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.7">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
       <c r="A144" s="7">
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.7">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
       <c r="A145" s="7">
         <v>144</v>
       </c>
@@ -2867,7 +2929,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="146" spans="1:2">
       <c r="A146" s="7">
         <v>145</v>
       </c>
@@ -2875,7 +2937,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="147" spans="1:2">
       <c r="A147" s="7">
         <v>146</v>
       </c>
@@ -2883,7 +2945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="148" spans="1:2">
       <c r="A148" s="7">
         <v>147</v>
       </c>
@@ -2891,7 +2953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="149" spans="1:2">
       <c r="A149" s="7">
         <v>148</v>
       </c>
@@ -2899,7 +2961,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="150" spans="1:2">
       <c r="A150" s="7">
         <v>149</v>
       </c>
@@ -2907,7 +2969,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="151" spans="1:2">
       <c r="A151" s="7">
         <v>150</v>
       </c>
@@ -2915,7 +2977,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="152" spans="1:2">
       <c r="A152" s="7">
         <v>151</v>
       </c>
@@ -2923,7 +2985,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="153" spans="1:2">
       <c r="A153" s="7">
         <v>152</v>
       </c>
@@ -2931,7 +2993,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="154" spans="1:2">
       <c r="A154" s="7">
         <v>153</v>
       </c>
@@ -2939,7 +3001,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="155" spans="1:2">
       <c r="A155" s="7">
         <v>154</v>
       </c>
@@ -2947,15 +3009,15 @@
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="156" spans="1:2">
       <c r="A156" s="7">
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.7">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
       <c r="A157" s="7">
         <v>156</v>
       </c>
@@ -2963,7 +3025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="158" spans="1:2">
       <c r="A158" s="7">
         <v>157</v>
       </c>
@@ -2971,135 +3033,135 @@
         <v>107</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="159" spans="1:2">
       <c r="A159" s="7">
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.7">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
       <c r="A160" s="7">
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.7">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
       <c r="A161" s="7">
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.7">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
       <c r="A162" s="7">
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="31.8" x14ac:dyDescent="0.7">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="22.15">
       <c r="A163" s="7">
         <v>162</v>
       </c>
       <c r="B163" s="17" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.7">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
       <c r="A164" s="7">
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.7">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" s="7">
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" s="7">
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.7">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
       <c r="A167" s="7">
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
       <c r="A168" s="7">
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.7">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
       <c r="A169" s="7">
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.7">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
       <c r="A170" s="7">
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.7">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
       <c r="A171" s="7">
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.7">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
       <c r="A172" s="7">
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.7">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
       <c r="A173" s="7">
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.7">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
       <c r="A174" s="7">
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.7">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
       <c r="A175" s="7">
         <v>174</v>
       </c>
@@ -3107,7 +3169,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="176" spans="1:2">
       <c r="A176" s="7">
         <v>175</v>
       </c>
@@ -3115,7 +3177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="177" spans="1:2">
       <c r="A177" s="7">
         <v>176</v>
       </c>
@@ -3123,7 +3185,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="178" spans="1:2">
       <c r="A178" s="7">
         <v>177</v>
       </c>
@@ -3131,7 +3193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="179" spans="1:2">
       <c r="A179" s="7">
         <v>178</v>
       </c>
@@ -3139,7 +3201,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="180" spans="1:2">
       <c r="A180" s="7">
         <v>179</v>
       </c>
@@ -3147,15 +3209,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="181" spans="1:2">
       <c r="A181" s="7">
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.7">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
       <c r="A182" s="7">
         <v>181</v>
       </c>
@@ -3163,7 +3225,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="183" spans="1:2">
       <c r="A183" s="7">
         <v>182</v>
       </c>
@@ -3171,7 +3233,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="184" spans="1:2">
       <c r="A184" s="7">
         <v>183</v>
       </c>
@@ -3179,7 +3241,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="185" spans="1:2" ht="30">
       <c r="A185" s="7">
         <v>184</v>
       </c>
@@ -3187,7 +3249,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="186" spans="1:2">
       <c r="A186" s="7">
         <v>185</v>
       </c>
@@ -3195,7 +3257,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="187" spans="1:2">
       <c r="A187" s="7">
         <v>186</v>
       </c>
@@ -3203,7 +3265,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="188" spans="1:2">
       <c r="A188" s="7">
         <v>187</v>
       </c>
@@ -3211,7 +3273,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="189" spans="1:2">
       <c r="A189" s="7">
         <v>188</v>
       </c>
@@ -3219,7 +3281,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="190" spans="1:2">
       <c r="A190" s="7">
         <v>189</v>
       </c>
@@ -3227,7 +3289,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="191" spans="1:2">
       <c r="A191" s="7">
         <v>190</v>
       </c>
@@ -3235,7 +3297,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="192" spans="1:2">
       <c r="A192" s="7">
         <v>191</v>
       </c>
@@ -3243,7 +3305,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="193" spans="1:2">
       <c r="A193" s="7">
         <v>192</v>
       </c>
@@ -3251,7 +3313,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="194" spans="1:2">
       <c r="A194" s="7">
         <v>193</v>
       </c>
@@ -3259,7 +3321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="195" spans="1:2">
       <c r="A195" s="7">
         <v>194</v>
       </c>
@@ -3267,15 +3329,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="196" spans="1:2">
       <c r="A196" s="7">
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.7">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
       <c r="A197" s="7">
         <v>196</v>
       </c>
@@ -3283,31 +3345,31 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="198" spans="1:2">
       <c r="A198" s="7">
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
       <c r="A199" s="7">
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.7">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
       <c r="A200" s="7">
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.7">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
       <c r="A201" s="7">
         <v>200</v>
       </c>
@@ -3315,7 +3377,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="202" spans="1:2">
       <c r="A202" s="7">
         <v>201</v>
       </c>
@@ -3323,15 +3385,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="203" spans="1:2">
       <c r="A203" s="7">
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.7">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
       <c r="A204" s="7">
         <v>203</v>
       </c>
@@ -3339,7 +3401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="205" spans="1:2">
       <c r="A205" s="7">
         <v>204</v>
       </c>
@@ -3347,7 +3409,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="206" spans="1:2">
       <c r="A206" s="7">
         <v>205</v>
       </c>
@@ -3355,7 +3417,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="207" spans="1:2">
       <c r="A207" s="7">
         <v>206</v>
       </c>
@@ -3363,7 +3425,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="208" spans="1:2">
       <c r="A208" s="7">
         <v>207</v>
       </c>
@@ -3371,15 +3433,15 @@
         <v>192</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="209" spans="1:2">
       <c r="A209" s="7">
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.7">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
       <c r="A210" s="7">
         <v>209</v>
       </c>
@@ -3387,7 +3449,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="211" spans="1:2">
       <c r="A211" s="7">
         <v>210</v>
       </c>
@@ -3395,7 +3457,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="212" spans="1:2">
       <c r="A212" s="7">
         <v>211</v>
       </c>
@@ -3403,7 +3465,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="213" spans="1:2">
       <c r="A213" s="7">
         <v>212</v>
       </c>
@@ -3411,7 +3473,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="214" spans="1:2">
       <c r="A214" s="7">
         <v>213</v>
       </c>
@@ -3419,7 +3481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="215" spans="1:2">
       <c r="A215" s="7">
         <v>214</v>
       </c>
@@ -3427,7 +3489,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="216" spans="1:2">
       <c r="A216" s="7">
         <v>215</v>
       </c>
@@ -3435,7 +3497,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="217" spans="1:2">
       <c r="A217" s="7">
         <v>216</v>
       </c>
@@ -3443,15 +3505,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="218" spans="1:2">
       <c r="A218" s="7">
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.7">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
       <c r="A219" s="7">
         <v>218</v>
       </c>
@@ -3459,7 +3521,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="220" spans="1:2">
       <c r="A220" s="7">
         <v>219</v>
       </c>
@@ -3467,7 +3529,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="221" spans="1:2">
       <c r="A221" s="7">
         <v>220</v>
       </c>
@@ -3475,23 +3537,23 @@
         <v>160</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="222" spans="1:2">
       <c r="A222" s="7">
         <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.7">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
       <c r="A223" s="7">
         <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.7">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
       <c r="A224" s="7">
         <v>223</v>
       </c>
@@ -3499,7 +3561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="225" spans="1:2">
       <c r="A225" s="7">
         <v>224</v>
       </c>
@@ -3507,7 +3569,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="226" spans="1:2">
       <c r="A226" s="7">
         <v>225</v>
       </c>
@@ -3515,7 +3577,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="227" spans="1:2">
       <c r="A227" s="7">
         <v>226</v>
       </c>
@@ -3523,23 +3585,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="228" spans="1:2">
       <c r="A228" s="7">
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.7">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
       <c r="A229" s="7">
         <v>228</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.7">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
       <c r="A230" s="7">
         <v>229</v>
       </c>
@@ -3547,7 +3609,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="231" spans="1:2">
       <c r="A231" s="7">
         <v>230</v>
       </c>
@@ -3555,7 +3617,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="232" spans="1:2">
       <c r="A232" s="7">
         <v>231</v>
       </c>
@@ -3563,7 +3625,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="233" spans="1:2">
       <c r="A233" s="7">
         <v>232</v>
       </c>
@@ -3571,71 +3633,71 @@
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="234" spans="1:2">
       <c r="A234" s="7">
         <v>233</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.7">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
       <c r="A235" s="7">
         <v>234</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.7">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
       <c r="A236" s="7">
         <v>235</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.7">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
       <c r="A237" s="7">
         <v>236</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.7">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
       <c r="A238" s="7">
         <v>237</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.7">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
       <c r="A239" s="7">
         <v>238</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
       <c r="A240" s="7">
         <v>239</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.7">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
       <c r="A241" s="7">
         <v>240</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.7">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
       <c r="A242" s="7">
         <v>241</v>
       </c>
@@ -3643,7 +3705,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="243" spans="1:2">
       <c r="A243" s="7">
         <v>242</v>
       </c>
@@ -3651,7 +3713,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="244" spans="1:2">
       <c r="A244" s="7">
         <v>243</v>
       </c>
@@ -3659,7 +3721,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="245" spans="1:2">
       <c r="A245" s="7">
         <v>244</v>
       </c>
@@ -3667,15 +3729,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="246" spans="1:2">
       <c r="A246" s="7">
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.7">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
       <c r="A247" s="7">
         <v>246</v>
       </c>
@@ -3683,7 +3745,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="248" spans="1:2">
       <c r="A248" s="7">
         <v>247</v>
       </c>
@@ -3691,7 +3753,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="249" spans="1:2">
       <c r="A249" s="7">
         <v>248</v>
       </c>
@@ -3699,15 +3761,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="250" spans="1:2">
       <c r="A250" s="7">
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.7">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
       <c r="A251" s="7">
         <v>250</v>
       </c>
@@ -3715,23 +3777,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="252" spans="1:2">
       <c r="A252" s="7">
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.7">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
       <c r="A253" s="7">
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.7">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
       <c r="A254" s="7">
         <v>253</v>
       </c>
@@ -3739,7 +3801,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="255" spans="1:2">
       <c r="A255" s="7">
         <v>254</v>
       </c>
@@ -3747,7 +3809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="256" spans="1:2">
       <c r="A256" s="7">
         <v>255</v>
       </c>
@@ -3755,87 +3817,87 @@
         <v>49</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="257" spans="1:2">
       <c r="A257" s="7">
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.7">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
       <c r="A258" s="7">
         <v>257</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.7">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
       <c r="A259" s="7">
         <v>258</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.7">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
       <c r="A260" s="7">
         <v>259</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.7">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
       <c r="A261" s="7">
         <v>260</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.7">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
       <c r="A262" s="7">
         <v>261</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
       <c r="A263" s="7">
         <v>262</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.7">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
       <c r="A264" s="7">
         <v>263</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.7">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
       <c r="A265" s="7">
         <v>264</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.7">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
       <c r="A266" s="7">
         <v>265</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.7">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
       <c r="A267" s="7">
         <v>266</v>
       </c>
@@ -3843,7 +3905,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="268" spans="1:2">
       <c r="A268" s="7">
         <v>267</v>
       </c>
@@ -3851,7 +3913,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="269" spans="1:2">
       <c r="A269" s="7">
         <v>268</v>
       </c>
@@ -3859,15 +3921,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="270" spans="1:2">
       <c r="A270" s="7">
         <v>269</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.7">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
       <c r="A271" s="7">
         <v>270</v>
       </c>
@@ -3875,7 +3937,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="272" spans="1:2">
       <c r="A272" s="7">
         <v>271</v>
       </c>
@@ -3883,7 +3945,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="273" spans="1:2">
       <c r="A273" s="7">
         <v>272</v>
       </c>
@@ -3891,7 +3953,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="274" spans="1:2">
       <c r="A274" s="7">
         <v>273</v>
       </c>
@@ -3899,7 +3961,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="275" spans="1:2">
       <c r="A275" s="7">
         <v>274</v>
       </c>
@@ -3907,7 +3969,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="276" spans="1:2">
       <c r="A276" s="7">
         <v>275</v>
       </c>
@@ -3915,7 +3977,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="277" spans="1:2">
       <c r="A277" s="7">
         <v>276</v>
       </c>
@@ -3923,7 +3985,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="278" spans="1:2">
       <c r="A278" s="7">
         <v>277</v>
       </c>
@@ -3931,7 +3993,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="279" spans="1:2">
       <c r="A279" s="7">
         <v>278</v>
       </c>
@@ -3939,15 +4001,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="280" spans="1:2">
       <c r="A280" s="7">
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.7">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
       <c r="A281" s="7">
         <v>280</v>
       </c>
@@ -3955,31 +4017,31 @@
         <v>101</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="282" spans="1:2">
       <c r="A282" s="7">
         <v>281</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.7">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
       <c r="A283" s="7">
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.7">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
       <c r="A284" s="7">
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.7">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
       <c r="A285" s="7">
         <v>284</v>
       </c>
@@ -3987,7 +4049,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="286" spans="1:2">
       <c r="A286" s="7">
         <v>285</v>
       </c>
@@ -3995,15 +4057,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="287" spans="1:2">
       <c r="A287" s="7">
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.7">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
       <c r="A288" s="7">
         <v>287</v>
       </c>
@@ -4011,7 +4073,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="289" spans="1:2">
       <c r="A289" s="7">
         <v>288</v>
       </c>
@@ -4019,7 +4081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="290" spans="1:2">
       <c r="A290" s="7">
         <v>289</v>
       </c>
@@ -4027,7 +4089,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="291" spans="1:2">
       <c r="A291" s="7">
         <v>290</v>
       </c>
@@ -4035,7 +4097,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="292" spans="1:2">
       <c r="A292" s="7">
         <v>291</v>
       </c>
@@ -4043,7 +4105,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="293" spans="1:2">
       <c r="A293" s="7">
         <v>292</v>
       </c>
@@ -4051,7 +4113,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="294" spans="1:2">
       <c r="A294" s="7">
         <v>293</v>
       </c>
@@ -4059,7 +4121,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="295" spans="1:2">
       <c r="A295" s="7">
         <v>294</v>
       </c>
@@ -4067,7 +4129,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="296" spans="1:2">
       <c r="A296" s="7">
         <v>295</v>
       </c>
@@ -4075,7 +4137,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="297" spans="1:2">
       <c r="A297" s="7">
         <v>296</v>
       </c>
@@ -4083,7 +4145,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="298" spans="1:2">
       <c r="A298" s="7">
         <v>297</v>
       </c>
@@ -4091,7 +4153,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="299" spans="1:2">
       <c r="A299" s="7">
         <v>298</v>
       </c>
@@ -4099,7 +4161,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="300" spans="1:2">
       <c r="A300" s="7">
         <v>299</v>
       </c>
@@ -4107,7 +4169,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="301" spans="1:2">
       <c r="A301" s="7">
         <v>300</v>
       </c>
@@ -4115,7 +4177,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="302" spans="1:2">
       <c r="A302" s="7">
         <v>301</v>
       </c>
@@ -4123,7 +4185,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="303" spans="1:2">
       <c r="A303" s="7">
         <v>302</v>
       </c>
@@ -4131,7 +4193,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="304" spans="1:2">
       <c r="A304" s="7">
         <v>303</v>
       </c>
@@ -4139,7 +4201,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="305" spans="1:2">
       <c r="A305" s="7">
         <v>304</v>
       </c>
@@ -4147,7 +4209,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="306" spans="1:2">
       <c r="A306" s="7">
         <v>305</v>
       </c>
@@ -4155,7 +4217,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="307" spans="1:2">
       <c r="A307" s="7">
         <v>306</v>
       </c>
@@ -4163,7 +4225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="308" spans="1:2">
       <c r="A308" s="7">
         <v>307</v>
       </c>
@@ -4171,7 +4233,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="309" spans="1:2">
       <c r="A309" s="7">
         <v>308</v>
       </c>
@@ -4179,7 +4241,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="310" spans="1:2">
       <c r="A310" s="7">
         <v>309</v>
       </c>
@@ -4187,7 +4249,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="311" spans="1:2">
       <c r="A311" s="7">
         <v>310</v>
       </c>
@@ -4195,7 +4257,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="312" spans="1:2">
       <c r="A312" s="7">
         <v>311</v>
       </c>
@@ -4203,7 +4265,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="313" spans="1:2">
       <c r="A313" s="7">
         <v>312</v>
       </c>
@@ -4211,7 +4273,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="314" spans="1:2">
       <c r="A314" s="7">
         <v>313</v>
       </c>
@@ -4219,7 +4281,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="315" spans="1:2">
       <c r="A315" s="7">
         <v>314</v>
       </c>
@@ -4227,7 +4289,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="316" spans="1:2">
       <c r="A316" s="7">
         <v>315</v>
       </c>
@@ -4235,7 +4297,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="317" spans="1:2">
       <c r="A317" s="7">
         <v>316</v>
       </c>
@@ -4243,7 +4305,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="318" spans="1:2">
       <c r="A318" s="7">
         <v>317</v>
       </c>
@@ -4251,7 +4313,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="319" spans="1:2">
       <c r="A319" s="7">
         <v>318</v>
       </c>
@@ -4259,7 +4321,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="320" spans="1:2">
       <c r="A320" s="7">
         <v>319</v>
       </c>
@@ -4267,7 +4329,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="321" spans="1:2">
       <c r="A321" s="7">
         <v>320</v>
       </c>
@@ -4275,7 +4337,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="322" spans="1:2">
       <c r="A322" s="7">
         <v>321</v>
       </c>
@@ -4283,15 +4345,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="323" spans="1:2">
       <c r="A323" s="7">
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.7">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
       <c r="A324" s="7">
         <v>323</v>
       </c>
@@ -4299,7 +4361,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="325" spans="1:2">
       <c r="A325" s="7">
         <v>324</v>
       </c>
@@ -4307,7 +4369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="326" spans="1:2">
       <c r="A326" s="7">
         <v>325</v>
       </c>
@@ -4315,7 +4377,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="327" spans="1:2">
       <c r="A327" s="7">
         <v>326</v>
       </c>
@@ -4323,7 +4385,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="328" spans="1:2">
       <c r="A328" s="7">
         <v>327</v>
       </c>
@@ -4331,79 +4393,79 @@
         <v>112</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="329" spans="1:2">
       <c r="A329" s="7">
         <v>328</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.7">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
       <c r="A330" s="7">
         <v>329</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.7">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
       <c r="A331" s="7">
         <v>330</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.7">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
       <c r="A332" s="7">
         <v>331</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.7">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
       <c r="A333" s="7">
         <v>332</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.7">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
       <c r="A334" s="7">
         <v>333</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.7">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
       <c r="A335" s="7">
         <v>334</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.7">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
       <c r="A336" s="7">
         <v>335</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.7">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
       <c r="A337" s="7">
         <v>336</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.7">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
       <c r="A338" s="7">
         <v>337</v>
       </c>
@@ -4411,7 +4473,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="339" spans="1:2">
       <c r="A339" s="7">
         <v>338</v>
       </c>
@@ -4419,7 +4481,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="340" spans="1:2">
       <c r="A340" s="7">
         <v>339</v>
       </c>
@@ -4427,7 +4489,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="341" spans="1:2">
       <c r="A341" s="7">
         <v>340</v>
       </c>
@@ -4435,7 +4497,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="342" spans="1:2">
       <c r="A342" s="7">
         <v>341</v>
       </c>
@@ -4443,7 +4505,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="343" spans="1:2">
       <c r="A343" s="7">
         <v>342</v>
       </c>
@@ -4451,7 +4513,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="344" spans="1:2">
       <c r="A344" s="7">
         <v>343</v>
       </c>
@@ -4459,7 +4521,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="345" spans="1:2">
       <c r="A345" s="7">
         <v>344</v>
       </c>
@@ -4467,7 +4529,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="346" spans="1:2">
       <c r="A346" s="7">
         <v>345</v>
       </c>
@@ -4475,7 +4537,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="347" spans="1:2">
       <c r="A347" s="7">
         <v>346</v>
       </c>
@@ -4483,7 +4545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="348" spans="1:2">
       <c r="A348" s="7">
         <v>347</v>
       </c>
@@ -4491,7 +4553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="349" spans="1:2">
       <c r="A349" s="7">
         <v>348</v>
       </c>
@@ -4499,7 +4561,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="350" spans="1:2">
       <c r="A350" s="7">
         <v>349</v>
       </c>
@@ -4507,7 +4569,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="351" spans="1:2">
       <c r="A351" s="7">
         <v>350</v>
       </c>
@@ -4515,7 +4577,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="352" spans="1:2">
       <c r="A352" s="7">
         <v>351</v>
       </c>
@@ -4523,7 +4585,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="353" spans="1:2">
       <c r="A353" s="7">
         <v>352</v>
       </c>
@@ -4531,23 +4593,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="354" spans="1:2">
       <c r="A354" s="7">
         <v>353</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.7">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
       <c r="A355" s="7">
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.7">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
       <c r="A356" s="7">
         <v>355</v>
       </c>
@@ -4555,7 +4617,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="357" spans="1:2">
       <c r="A357" s="7">
         <v>356</v>
       </c>
@@ -4563,7 +4625,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="358" spans="1:2">
       <c r="A358" s="7">
         <v>357</v>
       </c>
@@ -4571,7 +4633,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="359" spans="1:2">
       <c r="A359" s="7">
         <v>358</v>
       </c>
@@ -4579,15 +4641,15 @@
         <v>268</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="360" spans="1:2">
       <c r="A360" s="7">
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.7">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
       <c r="A361" s="7">
         <v>360</v>
       </c>
@@ -4595,31 +4657,31 @@
         <v>91</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="362" spans="1:2">
       <c r="A362" s="7">
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.7">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
       <c r="A363" s="7">
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.7">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
       <c r="A364" s="7">
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
       <c r="A365" s="7">
         <v>364</v>
       </c>
@@ -4627,23 +4689,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="366" spans="1:2">
       <c r="A366" s="7">
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.7">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
       <c r="A367" s="7">
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.7">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
       <c r="A368" s="7">
         <v>367</v>
       </c>
@@ -4651,7 +4713,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="369" spans="1:2">
       <c r="A369" s="7">
         <v>368</v>
       </c>
@@ -4659,7 +4721,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="370" spans="1:2">
       <c r="A370" s="7">
         <v>369</v>
       </c>
@@ -4667,7 +4729,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="371" spans="1:2">
       <c r="A371" s="7">
         <v>370</v>
       </c>
@@ -4675,7 +4737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="372" spans="1:2">
       <c r="A372" s="7">
         <v>371</v>
       </c>
@@ -4683,7 +4745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="373" spans="1:2">
       <c r="A373" s="7">
         <v>372</v>
       </c>
@@ -4691,7 +4753,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="374" spans="1:2">
       <c r="A374" s="7">
         <v>373</v>
       </c>
@@ -4699,7 +4761,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="375" spans="1:2">
       <c r="A375" s="7">
         <v>374</v>
       </c>
@@ -4707,7 +4769,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="376" spans="1:2">
       <c r="A376" s="7">
         <v>375</v>
       </c>
@@ -4715,31 +4777,31 @@
         <v>65</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="377" spans="1:2">
       <c r="A377" s="7">
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
       <c r="A378" s="7">
         <v>377</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
       <c r="A379" s="7">
         <v>378</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.7">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
       <c r="A380" s="7">
         <v>379</v>
       </c>
@@ -4747,7 +4809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="381" spans="1:2">
       <c r="A381" s="7">
         <v>380</v>
       </c>
@@ -4755,23 +4817,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="382" spans="1:2">
       <c r="A382" s="7">
         <v>381</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" ht="31.8" x14ac:dyDescent="0.7">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" ht="22.15">
       <c r="A383" s="7">
         <v>382</v>
       </c>
       <c r="B383" s="17" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.7">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
       <c r="A384" s="7">
         <v>383</v>
       </c>
@@ -4779,7 +4841,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="385" spans="1:2">
       <c r="A385" s="7">
         <v>384</v>
       </c>
@@ -4787,7 +4849,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="386" spans="1:2">
       <c r="A386" s="7">
         <v>385</v>
       </c>
@@ -4795,7 +4857,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="387" spans="1:2">
       <c r="A387" s="7">
         <v>386</v>
       </c>
@@ -4803,7 +4865,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="388" spans="1:2">
       <c r="A388" s="7">
         <v>387</v>
       </c>
@@ -4811,7 +4873,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="389" spans="1:2">
       <c r="A389" s="7">
         <v>388</v>
       </c>
@@ -4819,15 +4881,15 @@
         <v>260</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="390" spans="1:2">
       <c r="A390" s="7">
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.7">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
       <c r="A391" s="7">
         <v>390</v>
       </c>
@@ -4835,7 +4897,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="392" spans="1:2">
       <c r="A392" s="7">
         <v>391</v>
       </c>
@@ -4843,7 +4905,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="393" spans="1:2">
       <c r="A393" s="7">
         <v>392</v>
       </c>
@@ -4851,7 +4913,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="394" spans="1:2">
       <c r="A394" s="7">
         <v>393</v>
       </c>
@@ -4859,15 +4921,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="395" spans="1:2">
       <c r="A395" s="7">
         <v>394</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.7">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
       <c r="A396" s="7">
         <v>395</v>
       </c>
@@ -4875,7 +4937,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="397" spans="1:2">
       <c r="A397" s="7">
         <v>396</v>
       </c>
@@ -4883,7 +4945,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="398" spans="1:2">
       <c r="A398" s="7">
         <v>397</v>
       </c>
@@ -4891,7 +4953,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="399" spans="1:2">
       <c r="A399" s="7">
         <v>398</v>
       </c>
@@ -4899,23 +4961,23 @@
         <v>69</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="400" spans="1:2">
       <c r="A400" s="7">
         <v>399</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
       <c r="A401" s="7">
         <v>400</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.7">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
       <c r="A402" s="7">
         <v>401</v>
       </c>
@@ -4923,7 +4985,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="403" spans="1:2">
       <c r="A403" s="7">
         <v>402</v>
       </c>
@@ -4931,31 +4993,31 @@
         <v>44</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="404" spans="1:2">
       <c r="A404" s="7">
         <v>403</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.7">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
       <c r="A405" s="7">
         <v>404</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.7">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
       <c r="A406" s="7">
         <v>405</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.7">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
       <c r="A407" s="7">
         <v>406</v>
       </c>
@@ -4963,44 +5025,44 @@
         <v>253</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="408" spans="1:2">
       <c r="A408" s="7">
         <v>407</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.7">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
       <c r="A409" s="7">
         <v>408</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.7">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
       <c r="A410" s="7">
         <v>409</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.7">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
       <c r="A411" s="7">
         <v>410</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
       <c r="A412" s="7">
         <v>411</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5022,17 +5084,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -5040,31 +5102,31 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5072,7 +5134,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5080,71 +5142,71 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15">
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15">
       <c r="B14" s="13"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15">
       <c r="B15" s="13"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15">
       <c r="B16" s="13"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="15">
       <c r="B17" s="13"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15">
       <c r="B18" s="13"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="15">
       <c r="B26" s="13"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" ht="15">
       <c r="B29" s="13"/>
     </row>
   </sheetData>

</xml_diff>